<commit_message>
Actualizacion de mi log
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/logt1/forma-logt1-20095495.xlsx
+++ b/tspi/ciclo-1/logt1/forma-logt1-20095495.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgreyes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" tabRatio="400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="400"/>
   </bookViews>
   <sheets>
     <sheet name="LOGT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Video tutorial de Github.</t>
+  </si>
+  <si>
+    <t>Participé en el diagrama de caso de uso y escenarios de atributos de calidad</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK9"/>
+  <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" ref="E8:E9" si="0">((HOUR(C8)-HOUR(B8))*60)+(MINUTE(C8)-MINUTE(B8))-D8</f>
+        <f t="shared" ref="E8:E10" si="0">((HOUR(C8)-HOUR(B8))*60)+(MINUTE(C8)-MINUTE(B8))-D8</f>
         <v>45</v>
       </c>
       <c r="F8" s="4">
@@ -670,6 +673,30 @@
       </c>
       <c r="H9" s="5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>41892</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <f>((HOUR(C10)-HOUR(B10))*60)+(MINUTE(C10)-MINUTE(B10))-D10</f>
+        <v>140</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion del log y el task
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/logt1/forma-logt1-20095495.xlsx
+++ b/tspi/ciclo-1/logt1/forma-logt1-20095495.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-1\logt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Participé en el diagrama de caso de uso y escenarios de atributos de calidad</t>
+  </si>
+  <si>
+    <t>Reunión de equipo para discutir estados de las tareas del ciclo #1.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -208,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK10"/>
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,8 +605,8 @@
         <f>((HOUR(C6)-HOUR(B6))*60)+(MINUTE(C6)-MINUTE(B6))-D6</f>
         <v>20</v>
       </c>
-      <c r="F6" s="4">
-        <v>1</v>
+      <c r="F6" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>18</v>
@@ -621,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>15</v>
@@ -645,7 +654,7 @@
         <v>45</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>16</v>
@@ -669,7 +678,7 @@
         <v>90</v>
       </c>
       <c r="F9" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>17</v>
@@ -677,25 +686,49 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41892</v>
+        <v>41912</v>
       </c>
       <c r="B10" s="2">
+        <v>0.96875</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B11" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>0.93055555555555547</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
-        <f>((HOUR(C10)-HOUR(B10))*60)+(MINUTE(C10)-MINUTE(B10))-D10</f>
+      <c r="E11" s="3">
+        <f>((HOUR(C11)-HOUR(B11))*60)+(MINUTE(C11)-MINUTE(B11))-D11</f>
         <v>140</v>
       </c>
-      <c r="F10" s="4">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="F11" s="4">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>